<commit_message>
Add year 2019 to CPI reference file
</commit_message>
<xml_diff>
--- a/InputData/cpi.xlsx
+++ b/InputData/cpi.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbie\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-1.4.2-us - AEO Update\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74B894A-F356-4233-B257-22D3D9ACBC5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="135" windowWidth="20100" windowHeight="7410" activeTab="1"/>
+    <workbookView xWindow="5310" yWindow="1590" windowWidth="21660" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
   <si>
     <t>CPI Consumer Price Index</t>
   </si>
@@ -238,13 +249,16 @@
     <t>2018.............................................................................     .</t>
   </si>
   <si>
-    <t>https://www.bls.gov/cpi/tables/supplemental-files/historical-cpi-u-201812.pdf</t>
+    <t>2019.............................................................................     .</t>
+  </si>
+  <si>
+    <t>https://www.bls.gov/cpi/tables/supplemental-files/historical-cpi-u-201912.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -403,6 +417,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -438,6 +469,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -613,12 +661,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -637,7 +683,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -647,7 +693,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -677,7 +723,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -685,12 +731,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1228,7 +1272,7 @@
         <v>4.2</v>
       </c>
       <c r="G29" s="6">
-        <f t="shared" ref="G29:G56" si="0">$D$50/D29</f>
+        <f t="shared" ref="G29:G57" si="0">$D$50/D29</f>
         <v>1.6857121879588841</v>
       </c>
       <c r="M29" s="1"/>
@@ -1963,6 +2007,30 @@
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="4"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57">
+        <v>254.41200000000001</v>
+      </c>
+      <c r="C57">
+        <v>256.90300000000002</v>
+      </c>
+      <c r="D57">
+        <v>255.65700000000001</v>
+      </c>
+      <c r="E57">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F57">
+        <v>1.8</v>
+      </c>
+      <c r="G57" s="6">
+        <f t="shared" si="0"/>
+        <v>0.89805481563188172</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update cpi.xlsx with 2021 value
</commit_message>
<xml_diff>
--- a/InputData/cpi.xlsx
+++ b/InputData/cpi.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US_EPS\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59485A2-ADF5-4469-ABB4-3A063C7F174B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EBE68E1-0A35-441E-9C13-8DD4B5F8F5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="1620" windowWidth="12720" windowHeight="14955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
   <si>
     <t>CPI Consumer Price Index</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>2020............................................................................. .</t>
+  </si>
+  <si>
+    <t>2021............................................................................. .</t>
   </si>
 </sst>
 </file>
@@ -667,7 +670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -737,10 +740,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,7 +1282,7 @@
         <v>4.2</v>
       </c>
       <c r="G29" s="6">
-        <f t="shared" ref="G29:G57" si="0">$D$50/D29</f>
+        <f t="shared" ref="G29:G56" si="0">$D$50/D29</f>
         <v>1.6857121879588841</v>
       </c>
       <c r="M29" s="1"/>
@@ -2061,6 +2064,30 @@
       <c r="G58" s="6">
         <f>$D$50/D58</f>
         <v>0.88711067149387013</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59">
+        <v>266.23599999999999</v>
+      </c>
+      <c r="C59">
+        <v>275.70299999999997</v>
+      </c>
+      <c r="D59">
+        <v>270.97000000000003</v>
+      </c>
+      <c r="E59">
+        <v>7</v>
+      </c>
+      <c r="F59">
+        <v>4.7</v>
+      </c>
+      <c r="G59" s="6">
+        <f>$D$50/D59</f>
+        <v>0.84730412960844359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update cpi.xlsx with 2022 data
</commit_message>
<xml_diff>
--- a/InputData/cpi.xlsx
+++ b/InputData/cpi.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EBE68E1-0A35-441E-9C13-8DD4B5F8F5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660CF4A4-614C-46FA-A68D-A9FB7C757A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
   <si>
     <t>CPI Consumer Price Index</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Historical CPI-U</t>
   </si>
   <si>
-    <t>Page 4</t>
-  </si>
-  <si>
     <t>Historical Consumer Price Index for All Urban Consumers (CPI-U): U.S. city average, all items, index</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>–</t>
   </si>
   <si>
-    <t>https://www.bls.gov/cpi/tables/supplemental-files/historical-cpi-u-201912.pdf</t>
-  </si>
-  <si>
     <t>1968............................................................................. .</t>
   </si>
   <si>
@@ -259,6 +253,15 @@
   </si>
   <si>
     <t>2021............................................................................. .</t>
+  </si>
+  <si>
+    <t>https://www.bls.gov/cpi/tables/supplemental-files/historical-cpi-u-202212.pdf</t>
+  </si>
+  <si>
+    <t>Pages 4 and 5</t>
+  </si>
+  <si>
+    <t>2022............................................................................. .</t>
   </si>
 </sst>
 </file>
@@ -671,7 +674,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,12 +704,12 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -730,20 +733,17 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,17 +754,17 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -772,13 +772,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>8</v>
@@ -786,27 +786,27 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>34.799999999999997</v>
@@ -820,13 +820,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>36.700000000000003</v>
@@ -840,13 +840,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>38.799999999999997</v>
@@ -860,13 +860,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>40.5</v>
@@ -880,13 +880,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <v>41.8</v>
@@ -900,13 +900,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <v>44.4</v>
@@ -920,13 +920,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12">
         <v>49.3</v>
@@ -940,13 +940,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13">
         <v>53.8</v>
@@ -960,13 +960,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14">
         <v>56.9</v>
@@ -980,13 +980,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15">
         <v>60.6</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16">
         <v>65.2</v>
@@ -1020,13 +1020,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17">
         <v>72.599999999999994</v>
@@ -1040,13 +1040,13 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18">
         <v>82.4</v>
@@ -1060,13 +1060,13 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19">
         <v>90.9</v>
@@ -1080,13 +1080,13 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20">
         <v>96.5</v>
@@ -1100,13 +1100,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21">
         <v>99.6</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22">
         <v>102.9</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23">
         <v>106.6</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>109.1</v>
@@ -1180,7 +1180,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B25">
         <v>112.4</v>
@@ -1200,7 +1200,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B26">
         <v>116.8</v>
@@ -1220,7 +1220,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B27">
         <v>122.7</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B28">
         <v>128.69999999999999</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29">
         <v>135.19999999999999</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30">
         <v>139.19999999999999</v>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31">
         <v>143.69999999999999</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B32">
         <v>147.19999999999999</v>
@@ -1372,7 +1372,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B33">
         <v>151.5</v>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B34">
         <v>155.80000000000001</v>
@@ -1426,7 +1426,7 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B35">
         <v>159.9</v>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B36">
         <v>162.30000000000001</v>
@@ -1480,7 +1480,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B37">
         <v>165.4</v>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B38">
         <v>170.8</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B39">
         <v>176.6</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B40">
         <v>178.9</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B41">
         <v>183.3</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B42">
         <v>187.6</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B43">
         <v>193.2</v>
@@ -1669,7 +1669,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B44">
         <v>200.6</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B45">
         <v>205.709</v>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B46">
         <v>214.429</v>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B47">
         <v>213.13900000000001</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B48">
         <v>217.535</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B49">
         <v>223.59800000000001</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B50">
         <v>228.85</v>
@@ -1858,7 +1858,7 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B51">
         <v>232.36600000000001</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B52">
         <v>236.38399999999999</v>
@@ -1912,7 +1912,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B53">
         <v>236.26499999999999</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B54">
         <v>238.77799999999999</v>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B55">
         <v>244.07599999999999</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B56">
         <v>250.089</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B57">
         <v>254.41200000000001</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B58">
         <v>257.55700000000002</v>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B59">
         <v>266.23599999999999</v>
@@ -2089,6 +2089,33 @@
         <f>$D$50/D59</f>
         <v>0.84730412960844359</v>
       </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60">
+        <v>288.34699999999998</v>
+      </c>
+      <c r="C60">
+        <v>296.96300000000002</v>
+      </c>
+      <c r="D60">
+        <v>292.65499999999997</v>
+      </c>
+      <c r="E60">
+        <v>6.5</v>
+      </c>
+      <c r="F60">
+        <v>8</v>
+      </c>
+      <c r="G60" s="6">
+        <f>$D$50/D60</f>
+        <v>0.78452102304761584</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G62" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates cpi.xlsx with latest data
</commit_message>
<xml_diff>
--- a/InputData/cpi.xlsx
+++ b/InputData/cpi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660CF4A4-614C-46FA-A68D-A9FB7C757A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF94D8D-8031-494B-B04F-AF997E3AC321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14985" yWindow="1815" windowWidth="26730" windowHeight="20460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
   <si>
     <t>CPI Consumer Price Index</t>
   </si>
@@ -262,17 +262,22 @@
   </si>
   <si>
     <t>2022............................................................................. .</t>
+  </si>
+  <si>
+    <t>2023............................................................................. .</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="#0.0"/>
+    <numFmt numFmtId="167" formatCode="#0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +301,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -318,7 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -332,6 +343,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -351,9 +368,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -391,9 +408,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -426,26 +443,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -478,26 +478,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -673,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,8 +716,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{811BF41F-E918-49FA-B7DA-F8A221ADBF89}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -742,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,13 +1108,13 @@
       <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="7">
         <v>102.9</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="7">
         <v>104.9</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="7">
         <v>103.9</v>
       </c>
       <c r="E22">
@@ -1142,13 +1128,13 @@
       <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="7">
         <v>106.6</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="7">
         <v>108.5</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="7">
         <v>107.6</v>
       </c>
       <c r="E23">
@@ -1162,13 +1148,13 @@
       <c r="A24" t="s">
         <v>38</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="7">
         <v>109.1</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="7">
         <v>110.1</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="7">
         <v>109.6</v>
       </c>
       <c r="E24">
@@ -1182,13 +1168,13 @@
       <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="7">
         <v>112.4</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="7">
         <v>114.9</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="7">
         <v>113.6</v>
       </c>
       <c r="E25">
@@ -1202,13 +1188,13 @@
       <c r="A26" t="s">
         <v>40</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="7">
         <v>116.8</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="7">
         <v>119.7</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="7">
         <v>118.3</v>
       </c>
       <c r="E26">
@@ -1222,13 +1208,13 @@
       <c r="A27" t="s">
         <v>41</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="7">
         <v>122.7</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="7">
         <v>125.3</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="7">
         <v>124</v>
       </c>
       <c r="E27">
@@ -1242,13 +1228,13 @@
       <c r="A28" t="s">
         <v>42</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="7">
         <v>128.69999999999999</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="7">
         <v>132.6</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="7">
         <v>130.69999999999999</v>
       </c>
       <c r="E28">
@@ -1266,13 +1252,13 @@
       <c r="A29" t="s">
         <v>43</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="7">
         <v>135.19999999999999</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="7">
         <v>137.19999999999999</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="7">
         <v>136.19999999999999</v>
       </c>
       <c r="E29">
@@ -1293,13 +1279,13 @@
       <c r="A30" t="s">
         <v>44</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="7">
         <v>139.19999999999999</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="7">
         <v>141.4</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="7">
         <v>140.30000000000001</v>
       </c>
       <c r="E30">
@@ -1320,13 +1306,13 @@
       <c r="A31" t="s">
         <v>45</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="7">
         <v>143.69999999999999</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="7">
         <v>145.30000000000001</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="7">
         <v>144.5</v>
       </c>
       <c r="E31">
@@ -1347,13 +1333,13 @@
       <c r="A32" t="s">
         <v>46</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="7">
         <v>147.19999999999999</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="7">
         <v>149.30000000000001</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="7">
         <v>148.19999999999999</v>
       </c>
       <c r="E32">
@@ -1374,13 +1360,13 @@
       <c r="A33" t="s">
         <v>47</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="7">
         <v>151.5</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="7">
         <v>153.19999999999999</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="7">
         <v>152.4</v>
       </c>
       <c r="E33">
@@ -1401,13 +1387,13 @@
       <c r="A34" t="s">
         <v>48</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="7">
         <v>155.80000000000001</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="7">
         <v>157.9</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="7">
         <v>156.9</v>
       </c>
       <c r="E34">
@@ -1428,13 +1414,13 @@
       <c r="A35" t="s">
         <v>49</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="7">
         <v>159.9</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="7">
         <v>161.19999999999999</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="7">
         <v>160.5</v>
       </c>
       <c r="E35">
@@ -1455,13 +1441,13 @@
       <c r="A36" t="s">
         <v>50</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="7">
         <v>162.30000000000001</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="7">
         <v>163.69999999999999</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="7">
         <v>163</v>
       </c>
       <c r="E36">
@@ -1482,13 +1468,13 @@
       <c r="A37" t="s">
         <v>51</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="7">
         <v>165.4</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="7">
         <v>167.8</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="7">
         <v>166.6</v>
       </c>
       <c r="E37">
@@ -1509,13 +1495,13 @@
       <c r="A38" t="s">
         <v>52</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="7">
         <v>170.8</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="7">
         <v>173.6</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="7">
         <v>172.2</v>
       </c>
       <c r="E38">
@@ -1536,13 +1522,13 @@
       <c r="A39" t="s">
         <v>53</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="7">
         <v>176.6</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="7">
         <v>177.5</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="7">
         <v>177.1</v>
       </c>
       <c r="E39">
@@ -1563,13 +1549,13 @@
       <c r="A40" t="s">
         <v>54</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="7">
         <v>178.9</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="7">
         <v>180.9</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="7">
         <v>179.9</v>
       </c>
       <c r="E40">
@@ -1590,13 +1576,13 @@
       <c r="A41" t="s">
         <v>55</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="7">
         <v>183.3</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="7">
         <v>184.6</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="7">
         <v>184</v>
       </c>
       <c r="E41">
@@ -1617,13 +1603,13 @@
       <c r="A42" t="s">
         <v>56</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="7">
         <v>187.6</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="7">
         <v>190.2</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="7">
         <v>188.9</v>
       </c>
       <c r="E42">
@@ -1644,13 +1630,13 @@
       <c r="A43" t="s">
         <v>57</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="7">
         <v>193.2</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="7">
         <v>197.4</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="7">
         <v>195.3</v>
       </c>
       <c r="E43">
@@ -1671,13 +1657,13 @@
       <c r="A44" t="s">
         <v>58</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="7">
         <v>200.6</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="7">
         <v>202.6</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="7">
         <v>201.6</v>
       </c>
       <c r="E44">
@@ -1698,13 +1684,13 @@
       <c r="A45" t="s">
         <v>59</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="8">
         <v>205.709</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="8">
         <v>208.976</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="8">
         <v>207.34200000000001</v>
       </c>
       <c r="E45">
@@ -1725,13 +1711,13 @@
       <c r="A46" t="s">
         <v>60</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="8">
         <v>214.429</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="8">
         <v>216.17699999999999</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="8">
         <v>215.303</v>
       </c>
       <c r="E46">
@@ -1752,13 +1738,13 @@
       <c r="A47" t="s">
         <v>61</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="8">
         <v>213.13900000000001</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="8">
         <v>215.935</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="8">
         <v>214.53700000000001</v>
       </c>
       <c r="E47">
@@ -1779,13 +1765,13 @@
       <c r="A48" t="s">
         <v>62</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="8">
         <v>217.535</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="8">
         <v>218.57599999999999</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="8">
         <v>218.05600000000001</v>
       </c>
       <c r="E48">
@@ -1806,13 +1792,13 @@
       <c r="A49" t="s">
         <v>63</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="8">
         <v>223.59800000000001</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="8">
         <v>226.28</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="8">
         <v>224.93899999999999</v>
       </c>
       <c r="E49">
@@ -1833,13 +1819,13 @@
       <c r="A50" t="s">
         <v>64</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="8">
         <v>228.85</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="8">
         <v>230.33799999999999</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="8">
         <v>229.59399999999999</v>
       </c>
       <c r="E50">
@@ -1860,13 +1846,13 @@
       <c r="A51" t="s">
         <v>65</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="8">
         <v>232.36600000000001</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="8">
         <v>233.548</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="8">
         <v>232.95699999999999</v>
       </c>
       <c r="E51">
@@ -1887,13 +1873,13 @@
       <c r="A52" t="s">
         <v>66</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="8">
         <v>236.38399999999999</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="8">
         <v>237.08799999999999</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="8">
         <v>236.73599999999999</v>
       </c>
       <c r="E52">
@@ -1914,13 +1900,13 @@
       <c r="A53" t="s">
         <v>67</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="8">
         <v>236.26499999999999</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="8">
         <v>237.76900000000001</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="8">
         <v>237.017</v>
       </c>
       <c r="E53">
@@ -1941,13 +1927,13 @@
       <c r="A54" t="s">
         <v>68</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="8">
         <v>238.77799999999999</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="8">
         <v>241.23699999999999</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="8">
         <v>240.00700000000001</v>
       </c>
       <c r="E54">
@@ -1968,13 +1954,13 @@
       <c r="A55" t="s">
         <v>69</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="8">
         <v>244.07599999999999</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="8">
         <v>246.16300000000001</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="8">
         <v>245.12</v>
       </c>
       <c r="E55">
@@ -1995,13 +1981,13 @@
       <c r="A56" t="s">
         <v>70</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="8">
         <v>250.089</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="8">
         <v>252.125</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="8">
         <v>251.107</v>
       </c>
       <c r="E56">
@@ -2022,13 +2008,13 @@
       <c r="A57" t="s">
         <v>71</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="8">
         <v>254.41200000000001</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="8">
         <v>256.90300000000002</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="8">
         <v>255.65700000000001</v>
       </c>
       <c r="E57">
@@ -2046,13 +2032,13 @@
       <c r="A58" t="s">
         <v>72</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="8">
         <v>257.55700000000002</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="8">
         <v>260.065</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="8">
         <v>258.81099999999998</v>
       </c>
       <c r="E58">
@@ -2070,13 +2056,13 @@
       <c r="A59" t="s">
         <v>73</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="8">
         <v>266.23599999999999</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="8">
         <v>275.70299999999997</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="8">
         <v>270.97000000000003</v>
       </c>
       <c r="E59">
@@ -2094,13 +2080,13 @@
       <c r="A60" t="s">
         <v>76</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="8">
         <v>288.34699999999998</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="8">
         <v>296.96300000000002</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="8">
         <v>292.65499999999997</v>
       </c>
       <c r="E60">
@@ -2113,6 +2099,15 @@
         <f>$D$50/D60</f>
         <v>0.78452102304761584</v>
       </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="8">
+        <v>302.40800000000002</v>
+      </c>
+      <c r="G61" s="6"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G62" s="6"/>

</xml_diff>

<commit_message>
Update currency year to 2023
</commit_message>
<xml_diff>
--- a/InputData/cpi.xlsx
+++ b/InputData/cpi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF94D8D-8031-494B-B04F-AF997E3AC321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{698147E0-8145-46CB-AA60-1ED82BEC5780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14985" yWindow="1815" windowWidth="26730" windowHeight="20460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
   <si>
     <t>CPI Consumer Price Index</t>
   </si>
@@ -255,16 +255,13 @@
     <t>2021............................................................................. .</t>
   </si>
   <si>
-    <t>https://www.bls.gov/cpi/tables/supplemental-files/historical-cpi-u-202212.pdf</t>
-  </si>
-  <si>
-    <t>Pages 4 and 5</t>
-  </si>
-  <si>
     <t>2022............................................................................. .</t>
   </si>
   <si>
     <t>2023............................................................................. .</t>
+  </si>
+  <si>
+    <t>https://data.bls.gov/pdq/SurveyOutputServlet</t>
   </si>
 </sst>
 </file>
@@ -657,7 +654,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +674,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>2019</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -687,12 +684,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -716,11 +708,8 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{811BF41F-E918-49FA-B7DA-F8A221ADBF89}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -729,7 +718,7 @@
   <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2078,7 +2067,7 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B60" s="8">
         <v>288.34699999999998</v>
@@ -2102,12 +2091,21 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B61" s="8">
         <v>302.40800000000002</v>
       </c>
-      <c r="G61" s="6"/>
+      <c r="C61" s="8">
+        <v>306.99599999999998</v>
+      </c>
+      <c r="D61" s="8">
+        <v>304.702</v>
+      </c>
+      <c r="G61" s="6">
+        <f>$D$50/D61</f>
+        <v>0.75350342301658668</v>
+      </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G62" s="6"/>

</xml_diff>

<commit_message>
Update currency year to 2024
</commit_message>
<xml_diff>
--- a/InputData/cpi.xlsx
+++ b/InputData/cpi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{698147E0-8145-46CB-AA60-1ED82BEC5780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B39BD3-42AA-4DDE-BCD1-0F086876A133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
   <si>
     <t>CPI Consumer Price Index</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>https://data.bls.gov/pdq/SurveyOutputServlet</t>
+  </si>
+  <si>
+    <t>2024............................................................................. .</t>
   </si>
 </sst>
 </file>
@@ -653,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -717,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61:G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,7 +2111,22 @@
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G62" s="6"/>
+      <c r="A62" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62">
+        <v>312.14499999999998</v>
+      </c>
+      <c r="C62">
+        <v>315.233</v>
+      </c>
+      <c r="D62">
+        <v>313.68900000000002</v>
+      </c>
+      <c r="G62" s="6">
+        <f>$D$50/D62</f>
+        <v>0.73191600598044548</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>